<commit_message>
Update structure and tracking
</commit_message>
<xml_diff>
--- a/docs/FileTracking.xlsx
+++ b/docs/FileTracking.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intellij Workspaces\restaurant-booking\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ED3188-ED09-45DA-B2CF-0429D8081AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008AACD0-9FCC-4272-85C2-89905DDEDE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{862DB41C-269D-4ABF-BD43-F4A3086CBA33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{862DB41C-269D-4ABF-BD43-F4A3086CBA33}"/>
   </bookViews>
   <sheets>
-    <sheet name="File" sheetId="1" r:id="rId1"/>
-    <sheet name="Drop Down" sheetId="2" r:id="rId2"/>
+    <sheet name="Java Class" sheetId="1" r:id="rId1"/>
+    <sheet name="File" sheetId="3" r:id="rId2"/>
+    <sheet name="Drop Down" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>File name</t>
   </si>
@@ -110,13 +111,55 @@
   </si>
   <si>
     <t>Product</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>css</t>
+  </si>
+  <si>
+    <t>jsp</t>
+  </si>
+  <si>
+    <t>txt</t>
+  </si>
+  <si>
+    <t>servlet</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Staged</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Finalizing</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Revising</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>Trash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +199,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -177,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,11 +244,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -211,7 +289,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7FB368DF-A3D6-40CE-8A26-FACE824C54A2}" name="Table1" displayName="Table1" ref="A2:D20" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7FB368DF-A3D6-40CE-8A26-FACE824C54A2}" name="Table1" displayName="Table1" ref="A2:D20" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A2:D20" xr:uid="{7FB368DF-A3D6-40CE-8A26-FACE824C54A2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{746E9BCA-1533-47FD-949D-84F1E7E28028}" name="File name"/>
@@ -224,6 +302,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{656E4B6A-211D-491A-A282-649D1D7E85D2}" name="Table7" displayName="Table7" ref="A2:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0">
+  <autoFilter ref="A2:D9" xr:uid="{656E4B6A-211D-491A-A282-649D1D7E85D2}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{58468DA7-E8C5-4C29-95BC-D14E92E438AB}" name="File name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{652DB47E-7869-4264-A0D4-2875F8CEFC50}" name="Type" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{98C5711C-A316-4F7E-89B6-FF111F13169D}" name="Path" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{418A14FD-6945-4D48-9489-73B18DA9369B}" name="Status" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D68F1297-2F00-4250-A1EB-549D4D14FA7A}" name="Table3" displayName="Table3" ref="A1:A5" totalsRowShown="0">
   <autoFilter ref="A1:A5" xr:uid="{D68F1297-2F00-4250-A1EB-549D4D14FA7A}"/>
   <tableColumns count="1">
@@ -233,11 +324,31 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{614FDFF2-76D6-4D80-A588-802A6D8E30F8}" name="Table4" displayName="Table4" ref="C1:C5" totalsRowShown="0">
   <autoFilter ref="C1:C5" xr:uid="{614FDFF2-76D6-4D80-A588-802A6D8E30F8}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{E64ED2BD-04CB-4FCA-9694-BD0558D90B69}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B3C25920-748E-406B-A6C2-A08736824E68}" name="Table6" displayName="Table6" ref="E1:E6" totalsRowShown="0">
+  <autoFilter ref="E1:E6" xr:uid="{B3C25920-748E-406B-A6C2-A08736824E68}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{30571CA3-8C81-47FD-B4C8-A16B9FB82DA2}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{20EA184B-6A94-4A7B-9D32-101CB6CE09C1}" name="Table8" displayName="Table8" ref="G1:G10" totalsRowShown="0">
+  <autoFilter ref="G1:G10" xr:uid="{20EA184B-6A94-4A7B-9D32-101CB6CE09C1}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{9BC0035D-13AB-4925-B184-BCE403A48407}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -542,18 +653,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3ED72DF-229F-4F38-8935-14F5EF147E20}">
   <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="31.44140625" customWidth="1"/>
     <col min="3" max="3" width="47.109375" customWidth="1"/>
     <col min="4" max="4" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -581,7 +692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -595,7 +706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
@@ -609,7 +720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
@@ -623,7 +734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
@@ -637,7 +748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
@@ -651,7 +762,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -665,7 +776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -679,7 +790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -693,7 +804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -707,7 +818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -721,7 +832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -760,64 +871,224 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645C98AB-CCD4-47D6-957D-2F911B335D0F}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4105916B-1B64-43B4-8D4F-E79ECDB84F37}">
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A61DCFB8-679B-4459-A1BB-4387161A750C}">
+          <x14:formula1>
+            <xm:f>'Drop Down'!$E$2:$E$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:B9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1ECBCED-84D3-4FC9-9B2E-056551AF5523}">
+          <x14:formula1>
+            <xm:f>'Drop Down'!$G$2:$G$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645C98AB-CCD4-47D6-957D-2F911B335D0F}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="G10" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>